<commit_message>
More files and updates to slides
</commit_message>
<xml_diff>
--- a/Code/Coding together/manual_att.xlsx
+++ b/Code/Coding together/manual_att.xlsx
@@ -1,30 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scott_cunningham/Documents/Difference-in-Differences/Code/Coding together/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4BBAF3-2B18-6D4C-AB14-2F9043159E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C7667C-B268-5C44-94F1-FD601388C09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="50280" windowHeight="28300" activeTab="4" xr2:uid="{2EE18137-9303-494C-8C32-9DE193BE7F81}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="50280" windowHeight="27120" activeTab="3" xr2:uid="{2EE18137-9303-494C-8C32-9DE193BE7F81}"/>
   </bookViews>
   <sheets>
     <sheet name="Manual" sheetId="1" r:id="rId1"/>
     <sheet name="Overall ATT" sheetId="6" r:id="rId2"/>
     <sheet name="Not yet treated" sheetId="8" r:id="rId3"/>
-    <sheet name="Castle" sheetId="9" r:id="rId4"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet10" sheetId="10" r:id="rId6"/>
-    <sheet name="1986" sheetId="2" r:id="rId7"/>
-    <sheet name="1992" sheetId="3" r:id="rId8"/>
-    <sheet name="1998" sheetId="4" r:id="rId9"/>
-    <sheet name="2004" sheetId="5" r:id="rId10"/>
+    <sheet name="Example Dynamics" sheetId="11" r:id="rId4"/>
+    <sheet name="Castle" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId6"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId7"/>
+    <sheet name="1986" sheetId="2" r:id="rId8"/>
+    <sheet name="1992" sheetId="3" r:id="rId9"/>
+    <sheet name="1998" sheetId="4" r:id="rId10"/>
+    <sheet name="2004" sheetId="5" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="181">
   <si>
     <t>Treatment group</t>
   </si>
@@ -564,6 +565,27 @@
   </si>
   <si>
     <t>mu hat t+1</t>
+  </si>
+  <si>
+    <t>CS ATT</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>TWFE</t>
+  </si>
+  <si>
+    <t>Uses all data, but gets it wrong</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Only uses the colored and units to right as controls</t>
+  </si>
+  <si>
+    <t>t+7</t>
   </si>
 </sst>
 </file>
@@ -601,7 +623,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,8 +714,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -846,11 +898,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -892,7 +968,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -909,9 +984,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -949,6 +1021,37 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1467,6 +1570,188 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9CFAB-2F74-294C-962D-2EF94BD601E1}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1998</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>B2*6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1999</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C13" si="0">B3*6</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2001</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2002</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2003</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2004</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2005</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2006</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2007</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2008</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2009</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C2:C13)</f>
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC0B6FC2-9930-E046-9895-0CFC4EF2A4F2}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -2221,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B26958-D2FD-B340-96F0-C0F0E677AC3F}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView zoomScale="222" zoomScaleNormal="222" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2263,10 +2548,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="20">
-        <v>1986</v>
-      </c>
-      <c r="B2" s="28">
-        <v>10</v>
+        <v>1980</v>
+      </c>
+      <c r="B2" s="26">
+        <v>0</v>
       </c>
       <c r="C2" s="26">
         <v>0</v>
@@ -2274,31 +2559,21 @@
       <c r="D2" s="26">
         <v>0</v>
       </c>
-      <c r="E2" s="27">
-        <v>0</v>
-      </c>
-      <c r="H2" s="18">
-        <v>1986</v>
-      </c>
-      <c r="I2" s="31">
-        <v>10</v>
-      </c>
-      <c r="J2" s="36">
-        <v>0</v>
-      </c>
-      <c r="K2" s="36">
-        <v>0</v>
-      </c>
-      <c r="L2" s="37">
-        <v>0</v>
-      </c>
+      <c r="E2" s="26">
+        <v>0</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
-        <v>1987</v>
-      </c>
-      <c r="B3" s="28">
-        <v>20</v>
+        <v>1981</v>
+      </c>
+      <c r="B3" s="26">
+        <v>0</v>
       </c>
       <c r="C3" s="26">
         <v>0</v>
@@ -2306,31 +2581,21 @@
       <c r="D3" s="26">
         <v>0</v>
       </c>
-      <c r="E3" s="27">
-        <v>0</v>
-      </c>
-      <c r="H3" s="18">
-        <v>1987</v>
-      </c>
-      <c r="I3" s="32">
-        <v>20</v>
-      </c>
-      <c r="J3" s="38">
-        <v>0</v>
-      </c>
-      <c r="K3" s="38">
-        <v>0</v>
-      </c>
-      <c r="L3" s="39">
-        <v>0</v>
-      </c>
+      <c r="E3" s="26">
+        <v>0</v>
+      </c>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
-        <v>1988</v>
-      </c>
-      <c r="B4" s="28">
-        <v>30</v>
+        <v>1982</v>
+      </c>
+      <c r="B4" s="26">
+        <v>0</v>
       </c>
       <c r="C4" s="26">
         <v>0</v>
@@ -2338,34 +2603,21 @@
       <c r="D4" s="26">
         <v>0</v>
       </c>
-      <c r="E4" s="27">
-        <v>0</v>
-      </c>
-      <c r="H4" s="18">
-        <v>1988</v>
-      </c>
-      <c r="I4" s="32">
-        <v>30</v>
-      </c>
-      <c r="J4" s="38">
-        <v>0</v>
-      </c>
-      <c r="K4" s="38">
-        <v>0</v>
-      </c>
-      <c r="L4" s="39">
-        <v>0</v>
-      </c>
-      <c r="M4" t="s">
-        <v>108</v>
-      </c>
+      <c r="E4" s="26">
+        <v>0</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
-        <v>1989</v>
-      </c>
-      <c r="B5" s="28">
-        <v>40</v>
+        <v>1983</v>
+      </c>
+      <c r="B5" s="26">
+        <v>0</v>
       </c>
       <c r="C5" s="26">
         <v>0</v>
@@ -2373,34 +2625,21 @@
       <c r="D5" s="26">
         <v>0</v>
       </c>
-      <c r="E5" s="27">
-        <v>0</v>
-      </c>
-      <c r="H5" s="18">
-        <v>1989</v>
-      </c>
-      <c r="I5" s="32">
-        <v>40</v>
-      </c>
-      <c r="J5" s="38">
-        <v>0</v>
-      </c>
-      <c r="K5" s="38">
-        <v>0</v>
-      </c>
-      <c r="L5" s="39">
-        <v>0</v>
-      </c>
-      <c r="M5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E5" s="26">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
-        <v>1990</v>
-      </c>
-      <c r="B6" s="28">
-        <v>50</v>
+        <v>1984</v>
+      </c>
+      <c r="B6" s="26">
+        <v>0</v>
       </c>
       <c r="C6" s="26">
         <v>0</v>
@@ -2408,31 +2647,21 @@
       <c r="D6" s="26">
         <v>0</v>
       </c>
-      <c r="E6" s="27">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
-        <v>1990</v>
-      </c>
-      <c r="I6" s="32">
-        <v>50</v>
-      </c>
-      <c r="J6" s="38">
-        <v>0</v>
-      </c>
-      <c r="K6" s="38">
-        <v>0</v>
-      </c>
-      <c r="L6" s="39">
-        <v>0</v>
-      </c>
+      <c r="E6" s="26">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
-        <v>1991</v>
-      </c>
-      <c r="B7" s="28">
-        <v>60</v>
+        <v>1985</v>
+      </c>
+      <c r="B7" s="72">
+        <v>0</v>
       </c>
       <c r="C7" s="26">
         <v>0</v>
@@ -2440,34 +2669,24 @@
       <c r="D7" s="26">
         <v>0</v>
       </c>
-      <c r="E7" s="27">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>1991</v>
-      </c>
-      <c r="I7" s="32">
-        <v>60</v>
-      </c>
-      <c r="J7" s="38">
-        <v>0</v>
-      </c>
-      <c r="K7" s="38">
-        <v>0</v>
-      </c>
-      <c r="L7" s="39">
-        <v>0</v>
-      </c>
+      <c r="E7" s="26">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
-        <v>1992</v>
-      </c>
-      <c r="B8" s="28">
-        <v>70</v>
-      </c>
-      <c r="C8" s="30">
-        <v>8</v>
+        <v>1986</v>
+      </c>
+      <c r="B8" s="73">
+        <v>10</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
       </c>
       <c r="D8" s="26">
         <v>0</v>
@@ -2476,30 +2695,30 @@
         <v>0</v>
       </c>
       <c r="H8" s="18">
-        <v>1992</v>
-      </c>
-      <c r="I8" s="33">
-        <v>70</v>
-      </c>
-      <c r="J8" s="34">
-        <v>8</v>
-      </c>
-      <c r="K8" s="40">
-        <v>0</v>
-      </c>
-      <c r="L8" s="35">
+        <v>1986</v>
+      </c>
+      <c r="I8" s="30">
+        <v>10</v>
+      </c>
+      <c r="J8" s="35">
+        <v>0</v>
+      </c>
+      <c r="K8" s="35">
+        <v>0</v>
+      </c>
+      <c r="L8" s="36">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
-        <v>1993</v>
-      </c>
-      <c r="B9" s="28">
-        <v>80</v>
-      </c>
-      <c r="C9" s="28">
-        <v>16</v>
+        <v>1987</v>
+      </c>
+      <c r="B9" s="73">
+        <v>20</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
       </c>
       <c r="D9" s="26">
         <v>0</v>
@@ -2508,30 +2727,30 @@
         <v>0</v>
       </c>
       <c r="H9" s="18">
-        <v>1993</v>
-      </c>
-      <c r="I9" s="33">
-        <v>80</v>
-      </c>
-      <c r="J9" s="35">
-        <v>16</v>
-      </c>
-      <c r="K9" s="40">
-        <v>0</v>
-      </c>
-      <c r="L9" s="35">
+        <v>1987</v>
+      </c>
+      <c r="I9" s="31">
+        <v>20</v>
+      </c>
+      <c r="J9" s="37">
+        <v>0</v>
+      </c>
+      <c r="K9" s="37">
+        <v>0</v>
+      </c>
+      <c r="L9" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
-        <v>1994</v>
-      </c>
-      <c r="B10" s="28">
-        <v>90</v>
-      </c>
-      <c r="C10" s="28">
-        <v>24</v>
+        <v>1988</v>
+      </c>
+      <c r="B10" s="73">
+        <v>30</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0</v>
       </c>
       <c r="D10" s="26">
         <v>0</v>
@@ -2540,33 +2759,33 @@
         <v>0</v>
       </c>
       <c r="H10" s="18">
-        <v>1994</v>
-      </c>
-      <c r="I10" s="33">
-        <v>90</v>
-      </c>
-      <c r="J10" s="35">
-        <v>24</v>
-      </c>
-      <c r="K10" s="40">
-        <v>0</v>
-      </c>
-      <c r="L10" s="35">
+        <v>1988</v>
+      </c>
+      <c r="I10" s="31">
+        <v>30</v>
+      </c>
+      <c r="J10" s="37">
+        <v>0</v>
+      </c>
+      <c r="K10" s="37">
+        <v>0</v>
+      </c>
+      <c r="L10" s="38">
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
-        <v>1995</v>
-      </c>
-      <c r="B11" s="28">
-        <v>100</v>
-      </c>
-      <c r="C11" s="28">
-        <v>32</v>
+        <v>1989</v>
+      </c>
+      <c r="B11" s="73">
+        <v>40</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0</v>
       </c>
       <c r="D11" s="26">
         <v>0</v>
@@ -2575,33 +2794,33 @@
         <v>0</v>
       </c>
       <c r="H11" s="18">
-        <v>1995</v>
-      </c>
-      <c r="I11" s="33">
-        <v>100</v>
-      </c>
-      <c r="J11" s="35">
-        <v>32</v>
-      </c>
-      <c r="K11" s="40">
-        <v>0</v>
-      </c>
-      <c r="L11" s="35">
+        <v>1989</v>
+      </c>
+      <c r="I11" s="31">
+        <v>40</v>
+      </c>
+      <c r="J11" s="37">
+        <v>0</v>
+      </c>
+      <c r="K11" s="37">
+        <v>0</v>
+      </c>
+      <c r="L11" s="38">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
-        <v>1996</v>
-      </c>
-      <c r="B12" s="28">
-        <v>110</v>
-      </c>
-      <c r="C12" s="28">
-        <v>40</v>
+        <v>1990</v>
+      </c>
+      <c r="B12" s="73">
+        <v>50</v>
+      </c>
+      <c r="C12" s="26">
+        <v>0</v>
       </c>
       <c r="D12" s="26">
         <v>0</v>
@@ -2610,30 +2829,30 @@
         <v>0</v>
       </c>
       <c r="H12" s="18">
-        <v>1996</v>
-      </c>
-      <c r="I12" s="33">
-        <v>110</v>
-      </c>
-      <c r="J12" s="35">
-        <v>40</v>
-      </c>
-      <c r="K12" s="40">
-        <v>0</v>
-      </c>
-      <c r="L12" s="35">
+        <v>1990</v>
+      </c>
+      <c r="I12" s="31">
+        <v>50</v>
+      </c>
+      <c r="J12" s="37">
+        <v>0</v>
+      </c>
+      <c r="K12" s="37">
+        <v>0</v>
+      </c>
+      <c r="L12" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
-        <v>1997</v>
-      </c>
-      <c r="B13" s="28">
-        <v>120</v>
-      </c>
-      <c r="C13" s="28">
-        <v>48</v>
+        <v>1991</v>
+      </c>
+      <c r="B13" s="73">
+        <v>60</v>
+      </c>
+      <c r="C13" s="26">
+        <v>0</v>
       </c>
       <c r="D13" s="26">
         <v>0</v>
@@ -2642,537 +2861,735 @@
         <v>0</v>
       </c>
       <c r="H13" s="18">
-        <v>1997</v>
-      </c>
-      <c r="I13" s="33">
-        <v>120</v>
-      </c>
-      <c r="J13" s="35">
-        <v>48</v>
-      </c>
-      <c r="K13" s="40">
-        <v>0</v>
-      </c>
-      <c r="L13" s="35">
+        <v>1991</v>
+      </c>
+      <c r="I13" s="31">
+        <v>60</v>
+      </c>
+      <c r="J13" s="37">
+        <v>0</v>
+      </c>
+      <c r="K13" s="37">
+        <v>0</v>
+      </c>
+      <c r="L13" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
-        <v>1998</v>
-      </c>
-      <c r="B14" s="28">
-        <v>130</v>
-      </c>
-      <c r="C14" s="28">
-        <v>56</v>
-      </c>
-      <c r="D14" s="30">
-        <v>6</v>
+        <v>1992</v>
+      </c>
+      <c r="B14" s="73">
+        <v>70</v>
+      </c>
+      <c r="C14" s="75">
+        <v>8</v>
+      </c>
+      <c r="D14" s="26">
+        <v>0</v>
       </c>
       <c r="E14" s="27">
         <v>0</v>
       </c>
       <c r="H14" s="18">
-        <v>1998</v>
-      </c>
-      <c r="I14" s="41">
-        <v>130</v>
-      </c>
-      <c r="J14" s="42">
-        <v>56</v>
-      </c>
-      <c r="K14" s="43">
-        <v>6</v>
-      </c>
-      <c r="L14" s="42">
+        <v>1992</v>
+      </c>
+      <c r="I14" s="32">
+        <v>70</v>
+      </c>
+      <c r="J14" s="33">
+        <v>8</v>
+      </c>
+      <c r="K14" s="39">
+        <v>0</v>
+      </c>
+      <c r="L14" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
-        <v>1999</v>
-      </c>
-      <c r="B15" s="28">
-        <v>140</v>
-      </c>
-      <c r="C15" s="28">
-        <v>64</v>
-      </c>
-      <c r="D15" s="28">
-        <v>12</v>
+        <v>1993</v>
+      </c>
+      <c r="B15" s="73">
+        <v>80</v>
+      </c>
+      <c r="C15" s="76">
+        <v>16</v>
+      </c>
+      <c r="D15" s="26">
+        <v>0</v>
       </c>
       <c r="E15" s="27">
         <v>0</v>
       </c>
       <c r="H15" s="18">
-        <v>1999</v>
-      </c>
-      <c r="I15" s="41">
-        <v>140</v>
-      </c>
-      <c r="J15" s="42">
-        <v>64</v>
-      </c>
-      <c r="K15" s="42">
-        <v>12</v>
-      </c>
-      <c r="L15" s="42">
+        <v>1993</v>
+      </c>
+      <c r="I15" s="32">
+        <v>80</v>
+      </c>
+      <c r="J15" s="34">
+        <v>16</v>
+      </c>
+      <c r="K15" s="39">
+        <v>0</v>
+      </c>
+      <c r="L15" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
-        <v>2000</v>
-      </c>
-      <c r="B16" s="28">
-        <v>150</v>
-      </c>
-      <c r="C16" s="28">
-        <v>72</v>
-      </c>
-      <c r="D16" s="28">
-        <v>18</v>
+        <v>1994</v>
+      </c>
+      <c r="B16" s="73">
+        <v>90</v>
+      </c>
+      <c r="C16" s="76">
+        <v>24</v>
+      </c>
+      <c r="D16" s="26">
+        <v>0</v>
       </c>
       <c r="E16" s="27">
         <v>0</v>
       </c>
       <c r="H16" s="18">
-        <v>2000</v>
-      </c>
-      <c r="I16" s="41">
-        <v>150</v>
-      </c>
-      <c r="J16" s="42">
-        <v>72</v>
-      </c>
-      <c r="K16" s="42">
-        <v>18</v>
-      </c>
-      <c r="L16" s="42">
+        <v>1994</v>
+      </c>
+      <c r="I16" s="32">
+        <v>90</v>
+      </c>
+      <c r="J16" s="34">
+        <v>24</v>
+      </c>
+      <c r="K16" s="39">
+        <v>0</v>
+      </c>
+      <c r="L16" s="34">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
-        <v>2001</v>
-      </c>
-      <c r="B17" s="28">
-        <v>160</v>
-      </c>
-      <c r="C17" s="28">
-        <v>80</v>
-      </c>
-      <c r="D17" s="28">
-        <v>24</v>
+        <v>1995</v>
+      </c>
+      <c r="B17" s="73">
+        <v>100</v>
+      </c>
+      <c r="C17" s="76">
+        <v>32</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0</v>
       </c>
       <c r="E17" s="27">
         <v>0</v>
       </c>
       <c r="H17" s="18">
-        <v>2001</v>
-      </c>
-      <c r="I17" s="41">
-        <v>160</v>
-      </c>
-      <c r="J17" s="42">
-        <v>80</v>
-      </c>
-      <c r="K17" s="42">
-        <v>24</v>
-      </c>
-      <c r="L17" s="42">
+        <v>1995</v>
+      </c>
+      <c r="I17" s="32">
+        <v>100</v>
+      </c>
+      <c r="J17" s="34">
+        <v>32</v>
+      </c>
+      <c r="K17" s="39">
+        <v>0</v>
+      </c>
+      <c r="L17" s="34">
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
-        <v>2002</v>
-      </c>
-      <c r="B18" s="28">
-        <v>170</v>
-      </c>
-      <c r="C18" s="28">
-        <v>88</v>
-      </c>
-      <c r="D18" s="28">
-        <v>30</v>
+        <v>1996</v>
+      </c>
+      <c r="B18" s="73">
+        <v>110</v>
+      </c>
+      <c r="C18" s="76">
+        <v>40</v>
+      </c>
+      <c r="D18" s="26">
+        <v>0</v>
       </c>
       <c r="E18" s="27">
         <v>0</v>
       </c>
       <c r="H18" s="18">
-        <v>2002</v>
-      </c>
-      <c r="I18" s="41">
-        <v>170</v>
-      </c>
-      <c r="J18" s="42">
-        <v>88</v>
-      </c>
-      <c r="K18" s="42">
-        <v>30</v>
-      </c>
-      <c r="L18" s="42">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>114</v>
+        <v>1996</v>
+      </c>
+      <c r="I18" s="32">
+        <v>110</v>
+      </c>
+      <c r="J18" s="34">
+        <v>40</v>
+      </c>
+      <c r="K18" s="39">
+        <v>0</v>
+      </c>
+      <c r="L18" s="34">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
-        <v>2003</v>
-      </c>
-      <c r="B19" s="28">
-        <v>180</v>
-      </c>
-      <c r="C19" s="28">
-        <v>96</v>
-      </c>
-      <c r="D19" s="28">
-        <v>36</v>
+        <v>1997</v>
+      </c>
+      <c r="B19" s="73">
+        <v>120</v>
+      </c>
+      <c r="C19" s="76">
+        <v>48</v>
+      </c>
+      <c r="D19" s="26">
+        <v>0</v>
       </c>
       <c r="E19" s="27">
         <v>0</v>
       </c>
       <c r="H19" s="18">
-        <v>2003</v>
-      </c>
-      <c r="I19" s="41">
-        <v>180</v>
-      </c>
-      <c r="J19" s="42">
-        <v>96</v>
-      </c>
-      <c r="K19" s="42">
-        <v>36</v>
-      </c>
-      <c r="L19" s="42">
+        <v>1997</v>
+      </c>
+      <c r="I19" s="32">
+        <v>120</v>
+      </c>
+      <c r="J19" s="34">
+        <v>48</v>
+      </c>
+      <c r="K19" s="39">
+        <v>0</v>
+      </c>
+      <c r="L19" s="34">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
-        <v>2004</v>
-      </c>
-      <c r="B20" s="28">
-        <v>190</v>
-      </c>
-      <c r="C20" s="28">
-        <v>104</v>
-      </c>
-      <c r="D20" s="28">
-        <v>42</v>
-      </c>
-      <c r="E20" s="30">
-        <v>4</v>
-      </c>
-      <c r="H20" s="57">
-        <v>2004</v>
-      </c>
-      <c r="I20" s="58">
-        <v>190</v>
-      </c>
-      <c r="J20" s="59">
-        <v>104</v>
-      </c>
-      <c r="K20" s="59">
-        <v>42</v>
-      </c>
-      <c r="L20" s="60">
-        <v>4</v>
+        <v>1998</v>
+      </c>
+      <c r="B20" s="73">
+        <v>130</v>
+      </c>
+      <c r="C20" s="76">
+        <v>56</v>
+      </c>
+      <c r="D20" s="77">
+        <v>6</v>
+      </c>
+      <c r="E20" s="27">
+        <v>0</v>
+      </c>
+      <c r="H20" s="18">
+        <v>1998</v>
+      </c>
+      <c r="I20" s="40">
+        <v>130</v>
+      </c>
+      <c r="J20" s="41">
+        <v>56</v>
+      </c>
+      <c r="K20" s="42">
+        <v>6</v>
+      </c>
+      <c r="L20" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
-        <v>2005</v>
-      </c>
-      <c r="B21" s="28">
-        <v>200</v>
-      </c>
-      <c r="C21" s="28">
-        <v>112</v>
-      </c>
-      <c r="D21" s="28">
-        <v>48</v>
-      </c>
-      <c r="E21" s="28">
-        <v>8</v>
-      </c>
-      <c r="H21" s="57">
-        <v>2005</v>
-      </c>
-      <c r="I21" s="58">
-        <v>200</v>
-      </c>
-      <c r="J21" s="59">
-        <v>112</v>
-      </c>
-      <c r="K21" s="59">
-        <v>48</v>
-      </c>
-      <c r="L21" s="59">
-        <v>8</v>
+        <v>1999</v>
+      </c>
+      <c r="B21" s="73">
+        <v>140</v>
+      </c>
+      <c r="C21" s="76">
+        <v>64</v>
+      </c>
+      <c r="D21" s="78">
+        <v>12</v>
+      </c>
+      <c r="E21" s="27">
+        <v>0</v>
+      </c>
+      <c r="H21" s="18">
+        <v>1999</v>
+      </c>
+      <c r="I21" s="40">
+        <v>140</v>
+      </c>
+      <c r="J21" s="41">
+        <v>64</v>
+      </c>
+      <c r="K21" s="41">
+        <v>12</v>
+      </c>
+      <c r="L21" s="41">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
-        <v>2006</v>
-      </c>
-      <c r="B22" s="28">
-        <v>210</v>
-      </c>
-      <c r="C22" s="28">
-        <v>120</v>
-      </c>
-      <c r="D22" s="28">
-        <v>54</v>
-      </c>
-      <c r="E22" s="28">
-        <v>12</v>
-      </c>
-      <c r="H22" s="57">
-        <v>2006</v>
-      </c>
-      <c r="I22" s="58">
-        <v>210</v>
-      </c>
-      <c r="J22" s="59">
-        <v>120</v>
-      </c>
-      <c r="K22" s="59">
-        <v>54</v>
-      </c>
-      <c r="L22" s="59">
-        <v>12</v>
+        <v>2000</v>
+      </c>
+      <c r="B22" s="73">
+        <v>150</v>
+      </c>
+      <c r="C22" s="76">
+        <v>72</v>
+      </c>
+      <c r="D22" s="78">
+        <v>18</v>
+      </c>
+      <c r="E22" s="27">
+        <v>0</v>
+      </c>
+      <c r="H22" s="18">
+        <v>2000</v>
+      </c>
+      <c r="I22" s="40">
+        <v>150</v>
+      </c>
+      <c r="J22" s="41">
+        <v>72</v>
+      </c>
+      <c r="K22" s="41">
+        <v>18</v>
+      </c>
+      <c r="L22" s="41">
+        <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
-        <v>2007</v>
-      </c>
-      <c r="B23" s="28">
-        <v>220</v>
-      </c>
-      <c r="C23" s="28">
-        <v>128</v>
-      </c>
-      <c r="D23" s="28">
-        <v>60</v>
-      </c>
-      <c r="E23" s="28">
-        <v>16</v>
-      </c>
-      <c r="H23" s="57">
-        <v>2007</v>
-      </c>
-      <c r="I23" s="58">
-        <v>220</v>
-      </c>
-      <c r="J23" s="59">
-        <v>128</v>
-      </c>
-      <c r="K23" s="59">
-        <v>60</v>
-      </c>
-      <c r="L23" s="59">
-        <v>16</v>
+        <v>2001</v>
+      </c>
+      <c r="B23" s="73">
+        <v>160</v>
+      </c>
+      <c r="C23" s="76">
+        <v>80</v>
+      </c>
+      <c r="D23" s="78">
+        <v>24</v>
+      </c>
+      <c r="E23" s="27">
+        <v>0</v>
+      </c>
+      <c r="H23" s="18">
+        <v>2001</v>
+      </c>
+      <c r="I23" s="40">
+        <v>160</v>
+      </c>
+      <c r="J23" s="41">
+        <v>80</v>
+      </c>
+      <c r="K23" s="41">
+        <v>24</v>
+      </c>
+      <c r="L23" s="41">
+        <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
-        <v>2008</v>
-      </c>
-      <c r="B24" s="28">
-        <v>230</v>
-      </c>
-      <c r="C24" s="28">
-        <v>136</v>
-      </c>
-      <c r="D24" s="28">
-        <v>66</v>
-      </c>
-      <c r="E24" s="28">
-        <v>20</v>
-      </c>
-      <c r="H24" s="57">
-        <v>2008</v>
-      </c>
-      <c r="I24" s="58">
-        <v>230</v>
-      </c>
-      <c r="J24" s="59">
-        <v>136</v>
-      </c>
-      <c r="K24" s="59">
-        <v>66</v>
-      </c>
-      <c r="L24" s="59">
-        <v>20</v>
+        <v>2002</v>
+      </c>
+      <c r="B24" s="73">
+        <v>170</v>
+      </c>
+      <c r="C24" s="76">
+        <v>88</v>
+      </c>
+      <c r="D24" s="78">
+        <v>30</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0</v>
+      </c>
+      <c r="H24" s="18">
+        <v>2002</v>
+      </c>
+      <c r="I24" s="40">
+        <v>170</v>
+      </c>
+      <c r="J24" s="41">
+        <v>88</v>
+      </c>
+      <c r="K24" s="41">
+        <v>30</v>
+      </c>
+      <c r="L24" s="41">
+        <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
+        <v>2003</v>
+      </c>
+      <c r="B25" s="73">
+        <v>180</v>
+      </c>
+      <c r="C25" s="76">
+        <v>96</v>
+      </c>
+      <c r="D25" s="78">
+        <v>36</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="18">
+        <v>2003</v>
+      </c>
+      <c r="I25" s="40">
+        <v>180</v>
+      </c>
+      <c r="J25" s="41">
+        <v>96</v>
+      </c>
+      <c r="K25" s="41">
+        <v>36</v>
+      </c>
+      <c r="L25" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="80">
+        <v>2004</v>
+      </c>
+      <c r="B26" s="81">
+        <v>190</v>
+      </c>
+      <c r="C26" s="82">
+        <v>104</v>
+      </c>
+      <c r="D26" s="81">
+        <v>42</v>
+      </c>
+      <c r="E26" s="81">
+        <v>4</v>
+      </c>
+      <c r="H26" s="53">
+        <v>2004</v>
+      </c>
+      <c r="I26" s="54">
+        <v>190</v>
+      </c>
+      <c r="J26" s="55">
+        <v>104</v>
+      </c>
+      <c r="K26" s="55">
+        <v>42</v>
+      </c>
+      <c r="L26" s="56">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="83">
+        <v>2005</v>
+      </c>
+      <c r="B27" s="84">
+        <v>200</v>
+      </c>
+      <c r="C27" s="85">
+        <v>112</v>
+      </c>
+      <c r="D27" s="84">
+        <v>48</v>
+      </c>
+      <c r="E27" s="84">
+        <v>8</v>
+      </c>
+      <c r="H27" s="53">
+        <v>2005</v>
+      </c>
+      <c r="I27" s="54">
+        <v>200</v>
+      </c>
+      <c r="J27" s="55">
+        <v>112</v>
+      </c>
+      <c r="K27" s="55">
+        <v>48</v>
+      </c>
+      <c r="L27" s="55">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="83">
+        <v>2006</v>
+      </c>
+      <c r="B28" s="84">
+        <v>210</v>
+      </c>
+      <c r="C28" s="85">
+        <v>120</v>
+      </c>
+      <c r="D28" s="84">
+        <v>54</v>
+      </c>
+      <c r="E28" s="84">
+        <v>12</v>
+      </c>
+      <c r="H28" s="53">
+        <v>2006</v>
+      </c>
+      <c r="I28" s="54">
+        <v>210</v>
+      </c>
+      <c r="J28" s="55">
+        <v>120</v>
+      </c>
+      <c r="K28" s="55">
+        <v>54</v>
+      </c>
+      <c r="L28" s="55">
+        <v>12</v>
+      </c>
+      <c r="M28" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="83">
+        <v>2007</v>
+      </c>
+      <c r="B29" s="84">
+        <v>220</v>
+      </c>
+      <c r="C29" s="85">
+        <v>128</v>
+      </c>
+      <c r="D29" s="84">
+        <v>60</v>
+      </c>
+      <c r="E29" s="84">
+        <v>16</v>
+      </c>
+      <c r="H29" s="53">
+        <v>2007</v>
+      </c>
+      <c r="I29" s="54">
+        <v>220</v>
+      </c>
+      <c r="J29" s="55">
+        <v>128</v>
+      </c>
+      <c r="K29" s="55">
+        <v>60</v>
+      </c>
+      <c r="L29" s="55">
+        <v>16</v>
+      </c>
+      <c r="M29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="83">
+        <v>2008</v>
+      </c>
+      <c r="B30" s="84">
+        <v>230</v>
+      </c>
+      <c r="C30" s="85">
+        <v>136</v>
+      </c>
+      <c r="D30" s="84">
+        <v>66</v>
+      </c>
+      <c r="E30" s="84">
+        <v>20</v>
+      </c>
+      <c r="H30" s="53">
+        <v>2008</v>
+      </c>
+      <c r="I30" s="54">
+        <v>230</v>
+      </c>
+      <c r="J30" s="55">
+        <v>136</v>
+      </c>
+      <c r="K30" s="55">
+        <v>66</v>
+      </c>
+      <c r="L30" s="55">
+        <v>20</v>
+      </c>
+      <c r="M30" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="86">
         <v>2009</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B31" s="87">
         <v>240</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C31" s="88">
         <v>144</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D31" s="87">
         <v>72</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E31" s="87">
         <v>24</v>
       </c>
-      <c r="H25" s="57">
+      <c r="H31" s="53">
         <v>2009</v>
       </c>
-      <c r="I25" s="61">
+      <c r="I31" s="57">
         <v>240</v>
       </c>
-      <c r="J25" s="62">
+      <c r="J31" s="58">
         <v>144</v>
       </c>
-      <c r="K25" s="62">
+      <c r="K31" s="58">
         <v>72</v>
       </c>
-      <c r="L25" s="62">
+      <c r="L31" s="58">
         <v>24</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M31" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
+    <row r="32" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="46">
-        <f>AVERAGE(B2:B25)</f>
+      <c r="B32" s="47">
+        <f>AVERAGE(B8:B31)</f>
         <v>125</v>
       </c>
-      <c r="C26" s="47">
-        <f>AVERAGE(C8:C25)</f>
+      <c r="C32" s="79">
+        <f>AVERAGE(C14:C31)</f>
         <v>76</v>
       </c>
-      <c r="D26" s="47">
-        <f>AVERAGE(D14:D25)</f>
+      <c r="D32" s="79">
+        <f>AVERAGE(D20:D31)</f>
         <v>39</v>
       </c>
-      <c r="E26" s="48">
-        <f>AVERAGE(E20:E25)</f>
+      <c r="E32" s="43">
+        <f>AVERAGE(E26:E31)</f>
         <v>14</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H32" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I26" s="54">
-        <f>AVERAGE(I2:I19)</f>
+      <c r="I32" s="50">
+        <f>AVERAGE(I8:I25)</f>
         <v>95</v>
       </c>
-      <c r="J26" s="52">
-        <f>AVERAGE(J8:J19)</f>
+      <c r="J32" s="48">
+        <f>AVERAGE(J14:J25)</f>
         <v>52</v>
       </c>
-      <c r="K26" s="53">
-        <f>AVERAGE(K14:K19)</f>
+      <c r="K32" s="49">
+        <f>AVERAGE(K20:K25)</f>
         <v>21</v>
       </c>
-      <c r="L26" s="18" t="s">
+      <c r="L32" s="18" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="49" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="B27" s="50">
-        <f>AVERAGE(B2:B25,C8:C25,D14:D25,E20:E25)</f>
+      <c r="B33" s="46">
+        <f>AVERAGE(B8:B31,C14:C31,D20:D31,E26:E31)</f>
         <v>82</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G33" t="s">
         <v>124</v>
       </c>
-      <c r="H27" s="55" t="s">
+      <c r="H33" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="56">
-        <f>AVERAGE(I2:I19,J8:J19,K14:K19)</f>
+      <c r="I33" s="52">
+        <f>AVERAGE(I8:I25,J14:J25,K20:K25)</f>
         <v>68.333333333333329</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M33" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51" t="s">
+    <row r="34" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="44">
-        <f>AVERAGE(B26:E26)</f>
+      <c r="B34" s="43">
+        <f>AVERAGE(B32:E32)</f>
         <v>63.5</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G34" t="s">
         <v>124</v>
       </c>
-      <c r="H28" s="51" t="s">
+      <c r="H34" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="I28" s="44">
-        <f>AVERAGE(I26:K26)</f>
+      <c r="I34" s="43">
+        <f>AVERAGE(I32:K32)</f>
         <v>56</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M34" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="45"/>
-      <c r="M29" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="44"/>
+      <c r="M35" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>128</v>
       </c>
     </row>
@@ -3182,6 +3599,665 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{427D7F9C-7557-8540-96D6-26937F7166FA}">
+  <dimension ref="A1:H35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6:H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="89" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="90">
+        <v>1980</v>
+      </c>
+      <c r="B2" s="26">
+        <v>0</v>
+      </c>
+      <c r="C2" s="26">
+        <v>0</v>
+      </c>
+      <c r="D2" s="26">
+        <v>0</v>
+      </c>
+      <c r="E2" s="91">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="90">
+        <v>1981</v>
+      </c>
+      <c r="B3" s="26">
+        <v>0</v>
+      </c>
+      <c r="C3" s="26">
+        <v>0</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0</v>
+      </c>
+      <c r="E3" s="91">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="90">
+        <v>1982</v>
+      </c>
+      <c r="B4" s="26">
+        <v>0</v>
+      </c>
+      <c r="C4" s="26">
+        <v>0</v>
+      </c>
+      <c r="D4" s="26">
+        <v>0</v>
+      </c>
+      <c r="E4" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="90">
+        <v>1983</v>
+      </c>
+      <c r="B5" s="26">
+        <v>0</v>
+      </c>
+      <c r="C5" s="26">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0</v>
+      </c>
+      <c r="E5" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="90">
+        <v>1984</v>
+      </c>
+      <c r="B6" s="26">
+        <v>0</v>
+      </c>
+      <c r="C6" s="26">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0</v>
+      </c>
+      <c r="E6" s="91">
+        <v>0</v>
+      </c>
+      <c r="G6" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="H6" s="99">
+        <f>AVERAGE(B8,C14,D20)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="90">
+        <v>1985</v>
+      </c>
+      <c r="B7" s="26">
+        <v>0</v>
+      </c>
+      <c r="C7" s="26">
+        <v>0</v>
+      </c>
+      <c r="D7" s="26">
+        <v>0</v>
+      </c>
+      <c r="E7" s="91">
+        <v>0</v>
+      </c>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99">
+        <f t="shared" ref="H7:H10" si="0">AVERAGE(B9,C15,D21)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="90">
+        <v>1986</v>
+      </c>
+      <c r="B8" s="93">
+        <v>10</v>
+      </c>
+      <c r="C8" s="26">
+        <v>0</v>
+      </c>
+      <c r="D8" s="26">
+        <v>0</v>
+      </c>
+      <c r="E8" s="91">
+        <v>0</v>
+      </c>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="90">
+        <v>1987</v>
+      </c>
+      <c r="B9" s="94">
+        <v>20</v>
+      </c>
+      <c r="C9" s="26">
+        <v>0</v>
+      </c>
+      <c r="D9" s="26">
+        <v>0</v>
+      </c>
+      <c r="E9" s="91">
+        <v>0</v>
+      </c>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="90">
+        <v>1988</v>
+      </c>
+      <c r="B10" s="94">
+        <v>30</v>
+      </c>
+      <c r="C10" s="26">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26">
+        <v>0</v>
+      </c>
+      <c r="E10" s="91">
+        <v>0</v>
+      </c>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="90">
+        <v>1989</v>
+      </c>
+      <c r="B11" s="94">
+        <v>40</v>
+      </c>
+      <c r="C11" s="26">
+        <v>0</v>
+      </c>
+      <c r="D11" s="26">
+        <v>0</v>
+      </c>
+      <c r="E11" s="91">
+        <v>0</v>
+      </c>
+      <c r="G11" s="102" t="s">
+        <v>180</v>
+      </c>
+      <c r="H11" s="102">
+        <f>AVERAGE(B14,C20)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="90">
+        <v>1990</v>
+      </c>
+      <c r="B12" s="94">
+        <v>50</v>
+      </c>
+      <c r="C12" s="26">
+        <v>0</v>
+      </c>
+      <c r="D12" s="26">
+        <v>0</v>
+      </c>
+      <c r="E12" s="91">
+        <v>0</v>
+      </c>
+      <c r="H12" s="102">
+        <f t="shared" ref="H12:H16" si="1">AVERAGE(B15,C21)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="90">
+        <v>1991</v>
+      </c>
+      <c r="B13" s="94">
+        <v>60</v>
+      </c>
+      <c r="C13" s="26">
+        <v>0</v>
+      </c>
+      <c r="D13" s="26">
+        <v>0</v>
+      </c>
+      <c r="E13" s="91">
+        <v>0</v>
+      </c>
+      <c r="H13" s="102">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="90">
+        <v>1992</v>
+      </c>
+      <c r="B14" s="100">
+        <v>70</v>
+      </c>
+      <c r="C14" s="95">
+        <v>8</v>
+      </c>
+      <c r="D14" s="26">
+        <v>0</v>
+      </c>
+      <c r="E14" s="91">
+        <v>0</v>
+      </c>
+      <c r="H14" s="102">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="90">
+        <v>1993</v>
+      </c>
+      <c r="B15" s="100">
+        <v>80</v>
+      </c>
+      <c r="C15" s="96">
+        <v>16</v>
+      </c>
+      <c r="D15" s="26">
+        <v>0</v>
+      </c>
+      <c r="E15" s="91">
+        <v>0</v>
+      </c>
+      <c r="H15" s="102">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="90">
+        <v>1994</v>
+      </c>
+      <c r="B16" s="100">
+        <v>90</v>
+      </c>
+      <c r="C16" s="96">
+        <v>24</v>
+      </c>
+      <c r="D16" s="26">
+        <v>0</v>
+      </c>
+      <c r="E16" s="91">
+        <v>0</v>
+      </c>
+      <c r="H16" s="102">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="90">
+        <v>1995</v>
+      </c>
+      <c r="B17" s="100">
+        <v>100</v>
+      </c>
+      <c r="C17" s="96">
+        <v>32</v>
+      </c>
+      <c r="D17" s="26">
+        <v>0</v>
+      </c>
+      <c r="E17" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="90">
+        <v>1996</v>
+      </c>
+      <c r="B18" s="100">
+        <v>110</v>
+      </c>
+      <c r="C18" s="96">
+        <v>40</v>
+      </c>
+      <c r="D18" s="26">
+        <v>0</v>
+      </c>
+      <c r="E18" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="90">
+        <v>1997</v>
+      </c>
+      <c r="B19" s="100">
+        <v>120</v>
+      </c>
+      <c r="C19" s="96">
+        <v>48</v>
+      </c>
+      <c r="D19" s="26">
+        <v>0</v>
+      </c>
+      <c r="E19" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="90">
+        <v>1998</v>
+      </c>
+      <c r="B20" s="73">
+        <v>130</v>
+      </c>
+      <c r="C20" s="101">
+        <v>56</v>
+      </c>
+      <c r="D20" s="97">
+        <v>6</v>
+      </c>
+      <c r="E20" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="90">
+        <v>1999</v>
+      </c>
+      <c r="B21" s="73">
+        <v>140</v>
+      </c>
+      <c r="C21" s="101">
+        <v>64</v>
+      </c>
+      <c r="D21" s="98">
+        <v>12</v>
+      </c>
+      <c r="E21" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="90">
+        <v>2000</v>
+      </c>
+      <c r="B22" s="73">
+        <v>150</v>
+      </c>
+      <c r="C22" s="101">
+        <v>72</v>
+      </c>
+      <c r="D22" s="98">
+        <v>18</v>
+      </c>
+      <c r="E22" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="90">
+        <v>2001</v>
+      </c>
+      <c r="B23" s="73">
+        <v>160</v>
+      </c>
+      <c r="C23" s="101">
+        <v>80</v>
+      </c>
+      <c r="D23" s="98">
+        <v>24</v>
+      </c>
+      <c r="E23" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="90">
+        <v>2002</v>
+      </c>
+      <c r="B24" s="73">
+        <v>170</v>
+      </c>
+      <c r="C24" s="101">
+        <v>88</v>
+      </c>
+      <c r="D24" s="98">
+        <v>30</v>
+      </c>
+      <c r="E24" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="90">
+        <v>2003</v>
+      </c>
+      <c r="B25" s="74">
+        <v>180</v>
+      </c>
+      <c r="C25" s="101">
+        <v>96</v>
+      </c>
+      <c r="D25" s="98">
+        <v>36</v>
+      </c>
+      <c r="E25" s="91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="80">
+        <v>2004</v>
+      </c>
+      <c r="B26" s="81">
+        <v>190</v>
+      </c>
+      <c r="C26" s="81">
+        <v>104</v>
+      </c>
+      <c r="D26" s="81">
+        <v>42</v>
+      </c>
+      <c r="E26" s="82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="83">
+        <v>2005</v>
+      </c>
+      <c r="B27" s="84">
+        <v>200</v>
+      </c>
+      <c r="C27" s="84">
+        <v>112</v>
+      </c>
+      <c r="D27" s="84">
+        <v>48</v>
+      </c>
+      <c r="E27" s="85">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="83">
+        <v>2006</v>
+      </c>
+      <c r="B28" s="84">
+        <v>210</v>
+      </c>
+      <c r="C28" s="84">
+        <v>120</v>
+      </c>
+      <c r="D28" s="84">
+        <v>54</v>
+      </c>
+      <c r="E28" s="85">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="83">
+        <v>2007</v>
+      </c>
+      <c r="B29" s="84">
+        <v>220</v>
+      </c>
+      <c r="C29" s="84">
+        <v>128</v>
+      </c>
+      <c r="D29" s="84">
+        <v>60</v>
+      </c>
+      <c r="E29" s="85">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="83">
+        <v>2008</v>
+      </c>
+      <c r="B30" s="84">
+        <v>230</v>
+      </c>
+      <c r="C30" s="84">
+        <v>136</v>
+      </c>
+      <c r="D30" s="84">
+        <v>66</v>
+      </c>
+      <c r="E30" s="85">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="86">
+        <v>2009</v>
+      </c>
+      <c r="B31" s="87">
+        <v>240</v>
+      </c>
+      <c r="C31" s="87">
+        <v>144</v>
+      </c>
+      <c r="D31" s="87">
+        <v>72</v>
+      </c>
+      <c r="E31" s="88">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="92">
+        <f>AVERAGE(B8:B31)</f>
+        <v>125</v>
+      </c>
+      <c r="C32" s="92">
+        <f>AVERAGE(C14:C31)</f>
+        <v>76</v>
+      </c>
+      <c r="D32" s="92">
+        <f>AVERAGE(D20:D31)</f>
+        <v>39</v>
+      </c>
+      <c r="E32" s="43">
+        <f>AVERAGE(E26:E31)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="29">
+        <f>AVERAGE(B8:B31,C14:C31,D20:D31,E26:E31)</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="92">
+        <f>AVERAGE(B32:E32)</f>
+        <v>63.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>174</v>
+      </c>
+      <c r="B35">
+        <f>AVERAGE(B8:B25,C14:C25,D20:D25)</f>
+        <v>68.333333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8450D091-0CF3-4E4E-A0C2-7C7B515B5A3B}">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -3359,7 +4435,7 @@
       <c r="B8" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>134</v>
       </c>
       <c r="D8" s="27">
@@ -3557,11 +4633,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD037F86-B1EB-D145-9FD4-1C559B132293}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3589,7 +4665,7 @@
       <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="59" t="s">
         <v>153</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -3612,7 +4688,7 @@
       <c r="A2">
         <v>1986</v>
       </c>
-      <c r="B2" s="72">
+      <c r="B2" s="68">
         <v>10</v>
       </c>
       <c r="C2">
@@ -3624,10 +4700,10 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="G2" s="64">
+      <c r="G2" s="60">
         <v>1</v>
       </c>
-      <c r="H2" s="65">
+      <c r="H2" s="61">
         <v>0</v>
       </c>
       <c r="I2">
@@ -3645,7 +4721,7 @@
       <c r="A3">
         <v>1987</v>
       </c>
-      <c r="B3" s="73">
+      <c r="B3" s="69">
         <v>20</v>
       </c>
       <c r="C3">
@@ -3660,10 +4736,10 @@
       <c r="F3" t="s">
         <v>172</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="62">
         <v>1</v>
       </c>
-      <c r="H3" s="67" t="str">
+      <c r="H3" s="63" t="str">
         <f>"+1"</f>
         <v>+1</v>
       </c>
@@ -3682,7 +4758,7 @@
       <c r="A4">
         <v>1988</v>
       </c>
-      <c r="B4" s="74">
+      <c r="B4" s="70">
         <v>30</v>
       </c>
       <c r="C4">
@@ -3694,10 +4770,10 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="64">
         <v>2</v>
       </c>
-      <c r="H4" s="69" t="str">
+      <c r="H4" s="65" t="str">
         <f>"+2"</f>
         <v>+2</v>
       </c>
@@ -3710,7 +4786,7 @@
       <c r="A5">
         <v>1989</v>
       </c>
-      <c r="B5" s="74">
+      <c r="B5" s="70">
         <v>40</v>
       </c>
       <c r="C5">
@@ -3722,10 +4798,10 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="G5" s="70">
+      <c r="G5" s="66">
         <v>2</v>
       </c>
-      <c r="H5" s="71" t="str">
+      <c r="H5" s="67" t="str">
         <f>"+3"</f>
         <v>+3</v>
       </c>
@@ -3769,7 +4845,7 @@
       <c r="B7" s="10">
         <v>60</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="71">
         <v>0</v>
       </c>
       <c r="D7">
@@ -3786,7 +4862,7 @@
       <c r="B8" s="10">
         <v>70</v>
       </c>
-      <c r="C8" s="72">
+      <c r="C8" s="68">
         <v>8</v>
       </c>
       <c r="D8">
@@ -3806,7 +4882,7 @@
       <c r="B9" s="10">
         <v>80</v>
       </c>
-      <c r="C9" s="73">
+      <c r="C9" s="69">
         <v>16</v>
       </c>
       <c r="D9">
@@ -3829,7 +4905,7 @@
       <c r="B10" s="10">
         <v>90</v>
       </c>
-      <c r="C10" s="74">
+      <c r="C10" s="70">
         <v>24</v>
       </c>
       <c r="D10">
@@ -3849,7 +4925,7 @@
       <c r="B11" s="10">
         <v>100</v>
       </c>
-      <c r="C11" s="74">
+      <c r="C11" s="70">
         <v>32</v>
       </c>
       <c r="D11">
@@ -3889,7 +4965,7 @@
       <c r="C13" s="10">
         <v>48</v>
       </c>
-      <c r="D13" s="75">
+      <c r="D13" s="71">
         <v>0</v>
       </c>
       <c r="E13">
@@ -3909,7 +4985,7 @@
       <c r="C14" s="10">
         <v>56</v>
       </c>
-      <c r="D14" s="72">
+      <c r="D14" s="68">
         <v>6</v>
       </c>
       <c r="E14">
@@ -3929,7 +5005,7 @@
       <c r="C15" s="10">
         <v>64</v>
       </c>
-      <c r="D15" s="73">
+      <c r="D15" s="69">
         <v>12</v>
       </c>
       <c r="E15">
@@ -3949,7 +5025,7 @@
       <c r="C16" s="10">
         <v>72</v>
       </c>
-      <c r="D16" s="74">
+      <c r="D16" s="70">
         <v>18</v>
       </c>
       <c r="E16">
@@ -3969,7 +5045,7 @@
       <c r="C17" s="10">
         <v>80</v>
       </c>
-      <c r="D17" s="74">
+      <c r="D17" s="70">
         <v>24</v>
       </c>
       <c r="E17">
@@ -4009,7 +5085,7 @@
       <c r="D19" s="10">
         <v>36</v>
       </c>
-      <c r="E19" s="75">
+      <c r="E19" s="71">
         <v>0</v>
       </c>
       <c r="H19" t="s">
@@ -4029,10 +5105,10 @@
       <c r="D20" s="10">
         <v>42</v>
       </c>
-      <c r="E20" s="72">
+      <c r="E20" s="68">
         <v>4</v>
       </c>
-      <c r="F20" s="45"/>
+      <c r="F20" s="44"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -4047,10 +5123,10 @@
       <c r="D21" s="10">
         <v>48</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="69">
         <v>8</v>
       </c>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="44" t="s">
         <v>172</v>
       </c>
       <c r="G21" t="s">
@@ -4076,10 +5152,10 @@
       <c r="D22" s="10">
         <v>54</v>
       </c>
-      <c r="E22" s="74">
+      <c r="E22" s="70">
         <v>12</v>
       </c>
-      <c r="F22" s="45"/>
+      <c r="F22" s="44"/>
       <c r="H22" s="15" t="s">
         <v>71</v>
       </c>
@@ -4100,10 +5176,10 @@
       <c r="D23" s="10">
         <v>60</v>
       </c>
-      <c r="E23" s="74">
+      <c r="E23" s="70">
         <v>16</v>
       </c>
-      <c r="F23" s="45"/>
+      <c r="F23" s="44"/>
       <c r="H23" t="s">
         <v>72</v>
       </c>
@@ -4124,7 +5200,7 @@
       <c r="E24" s="13">
         <v>20</v>
       </c>
-      <c r="F24" s="45"/>
+      <c r="F24" s="44"/>
       <c r="H24" t="s">
         <v>92</v>
       </c>
@@ -4215,7 +5291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DB1483-9CC9-2F4E-83A7-AE1B5CB4D0D4}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -4321,7 +5397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9A91786-16AB-C24D-8ACB-8D903D480A4A}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -4660,7 +5736,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E7CEF5-FDCD-594B-9FB3-DB278821F2A8}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -4912,186 +5988,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A9CFAB-2F74-294C-962D-2EF94BD601E1}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView zoomScale="271" zoomScaleNormal="271" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1998</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <f>B2*6</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1999</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C13" si="0">B3*6</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2000</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2001</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>2002</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2003</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2004</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2005</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>2006</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2007</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2008</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2009</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15">
-        <f>AVERAGE(C2:C13)</f>
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>